<commit_message>
added logging and output file
</commit_message>
<xml_diff>
--- a/sudoku_solver_analysis.xlsx
+++ b/sudoku_solver_analysis.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikram Vasudevan\Documents\Vikram\Official\Study\python\sudoku_solver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6347680D-F716-4B11-B664-7D8D73784882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0483F70A-9427-454C-9091-303998FA228A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB87C03A-0C91-4F56-A7E2-3B90D592D541}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{DB87C03A-0C91-4F56-A7E2-3B90D592D541}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Unsolvable" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -178,7 +179,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -490,7 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD6DA3A8-84E4-4A29-AF13-9CF5D18A4D92}">
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N1" sqref="N1:V9"/>
     </sheetView>
   </sheetViews>
@@ -1491,4 +1503,285 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6E5090-91F9-41CA-B2A1-40A770A18861}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>2</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>9</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:I9">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added more complex examples
</commit_message>
<xml_diff>
--- a/sudoku_solver_analysis.xlsx
+++ b/sudoku_solver_analysis.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikram Vasudevan\Documents\Vikram\Official\Study\python\sudoku_solver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC8A594-B04E-41DD-9B53-8333D92AE889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5547E23-662A-4E77-93EC-7F1D4D8D433A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB87C03A-0C91-4F56-A7E2-3B90D592D541}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{DB87C03A-0C91-4F56-A7E2-3B90D592D541}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Unsolvable" sheetId="3" r:id="rId3"/>
+    <sheet name="Grid Converter" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -47,6 +48,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -175,9 +182,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,7 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD6DA3A8-84E4-4A29-AF13-9CF5D18A4D92}">
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T7" sqref="T7:V9"/>
     </sheetView>
   </sheetViews>
@@ -602,7 +607,7 @@
         <f>N1+9</f>
         <v>9</v>
       </c>
-      <c r="O2" s="11">
+      <c r="O2" s="4">
         <f>N2+1</f>
         <v>10</v>
       </c>
@@ -614,7 +619,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="R2" s="11">
+      <c r="R2" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -626,7 +631,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="U2" s="11">
+      <c r="U2" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -797,7 +802,7 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="4">
         <f t="shared" ref="O5:V5" si="4">N5+1</f>
         <v>37</v>
       </c>
@@ -809,7 +814,7 @@
         <f t="shared" si="4"/>
         <v>39</v>
       </c>
-      <c r="R5" s="11">
+      <c r="R5" s="4">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
@@ -821,7 +826,7 @@
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="U5" s="11">
+      <c r="U5" s="4">
         <f t="shared" si="4"/>
         <v>43</v>
       </c>
@@ -992,7 +997,7 @@
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="4">
         <f t="shared" ref="O8:V8" si="7">N8+1</f>
         <v>64</v>
       </c>
@@ -1004,7 +1009,7 @@
         <f t="shared" si="7"/>
         <v>66</v>
       </c>
-      <c r="R8" s="11">
+      <c r="R8" s="4">
         <f t="shared" si="7"/>
         <v>67</v>
       </c>
@@ -1016,7 +1021,7 @@
         <f t="shared" si="7"/>
         <v>69</v>
       </c>
-      <c r="U8" s="11">
+      <c r="U8" s="4">
         <f t="shared" si="7"/>
         <v>70</v>
       </c>
@@ -1787,4 +1792,394 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27A290B-B1DA-418B-93C5-3BE88B782447}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>8</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>2</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="K1" s="11" t="str">
+        <f>_xlfn.TEXTJOIN(",",FALSE,A1:I1)</f>
+        <v>0,0,0,8,0,0,5,2,0</v>
+      </c>
+      <c r="L1" s="11" t="str">
+        <f>_xlfn.CONCAT("[",K1,"]")</f>
+        <v>[0,0,0,8,0,0,5,2,0]</v>
+      </c>
+      <c r="M1" s="11" t="str">
+        <f>_xlfn.CONCAT(L1,",")</f>
+        <v>[0,0,0,8,0,0,5,2,0],</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="11" t="str">
+        <f t="shared" ref="K2:K9" si="0">_xlfn.TEXTJOIN(",",FALSE,A2:I2)</f>
+        <v>0,0,0,0,7,0,0,0,0</v>
+      </c>
+      <c r="L2" s="11" t="str">
+        <f t="shared" ref="L2:L9" si="1">_xlfn.CONCAT("[",K2,"]")</f>
+        <v>[0,0,0,0,7,0,0,0,0]</v>
+      </c>
+      <c r="M2" s="11" t="str">
+        <f t="shared" ref="M2:M9" si="2">_xlfn.CONCAT(L2,",")</f>
+        <v>[0,0,0,0,7,0,0,0,0],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0,0,0,9,0,5,1,4,0</v>
+      </c>
+      <c r="L3" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>[0,0,0,9,0,5,1,4,0]</v>
+      </c>
+      <c r="M3" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>[0,0,0,9,0,5,1,4,0],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="K4" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0,0,4,0,5,0,2,0,8</v>
+      </c>
+      <c r="L4" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>[0,0,4,0,5,0,2,0,8]</v>
+      </c>
+      <c r="M4" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>[0,0,4,0,5,0,2,0,8],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>9,0,0,0,0,4,0,3,0</v>
+      </c>
+      <c r="L5" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>[9,0,0,0,0,4,0,3,0]</v>
+      </c>
+      <c r="M5" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>[9,0,0,0,0,4,0,3,0],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0,0,6,0,0,0,0,0,0</v>
+      </c>
+      <c r="L6" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>[0,0,6,0,0,0,0,0,0]</v>
+      </c>
+      <c r="M6" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>[0,0,6,0,0,0,0,0,0],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="K7" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0,0,0,0,6,9,0,0,3</v>
+      </c>
+      <c r="L7" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>[0,0,0,0,6,9,0,0,3]</v>
+      </c>
+      <c r="M7" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>[0,0,0,0,6,9,0,0,3],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>7,8,1,0,0,0,0,0,0</v>
+      </c>
+      <c r="L8" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>[7,8,1,0,0,0,0,0,0]</v>
+      </c>
+      <c r="M8" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>[7,8,1,0,0,0,0,0,0],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0,6,0,2,0,0,0,0,0</v>
+      </c>
+      <c r="L9" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>[0,6,0,2,0,0,0,0,0]</v>
+      </c>
+      <c r="M9" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>[0,6,0,2,0,0,0,0,0],</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>